<commit_message>
Addressing reviewer comments and updating figures
</commit_message>
<xml_diff>
--- a/Manuscript_Snips/Example_Excel_input.xlsx
+++ b/Manuscript_Snips/Example_Excel_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - University of Cambridge\Postdoc\PYthonBarometers\ClassicalThermometers_20210114T090546Z_001\ClassicalThermometers\Benchmarking\Tidy_Scripts_To_Share\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Postdoc\PyMME\MyBarometers\Thermobar_outer\Manuscript_Snips\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20D124A-0F96-4D00-BF13-FE5D1D009752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A942E426-23B5-438B-91BF-EA0213ECBBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{CC070845-6079-4A12-A7B6-8180E8A85D66}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{CC070845-6079-4A12-A7B6-8180E8A85D66}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Sample_ID_Liq</t>
   </si>
@@ -120,6 +120,33 @@
   </si>
   <si>
     <t>Cr2O3_Plag</t>
+  </si>
+  <si>
+    <t>K46</t>
+  </si>
+  <si>
+    <t>K49</t>
+  </si>
+  <si>
+    <t>Sample_ID_Plag</t>
+  </si>
+  <si>
+    <t>plg10</t>
+  </si>
+  <si>
+    <t>K33_plg1_spot3</t>
+  </si>
+  <si>
+    <t>K34_plg2</t>
+  </si>
+  <si>
+    <t>K44_plg1</t>
+  </si>
+  <si>
+    <t>K46_plg2</t>
+  </si>
+  <si>
+    <t>K49_plg1</t>
   </si>
 </sst>
 </file>
@@ -175,7 +202,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -184,6 +210,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -500,334 +529,631 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7261C75F-8A1F-44F1-BB62-20C732642454}">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.6328125" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" customWidth="1"/>
-    <col min="18" max="18" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" customWidth="1"/>
+    <col min="10" max="11" width="8.7265625" customWidth="1"/>
+    <col min="16" max="16" width="12.1796875" customWidth="1"/>
+    <col min="17" max="17" width="13.6328125" customWidth="1"/>
+    <col min="18" max="18" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="Z1" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>49.1</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>3.22</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>14.4</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>14.8</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0.15</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>3.2</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>3.2</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>6.72</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>3.34</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="3">
         <v>1.7</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="4">
-        <v>0</v>
-      </c>
-      <c r="N2" s="4">
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
         <v>3</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="3">
         <v>1350</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="4">
         <v>57.3</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="Q2" s="4">
         <v>0.09</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="4">
         <v>26.6</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="4">
         <v>0.43</v>
       </c>
-      <c r="T2" s="5">
-        <v>0</v>
-      </c>
-      <c r="U2" s="5">
+      <c r="T2" s="4">
+        <v>0</v>
+      </c>
+      <c r="U2" s="4">
         <v>0.03</v>
       </c>
-      <c r="V2" s="5">
+      <c r="V2" s="4">
         <v>8.33</v>
       </c>
-      <c r="W2" s="5">
+      <c r="W2" s="4">
         <v>6.11</v>
       </c>
-      <c r="X2" s="5">
+      <c r="X2" s="4">
         <v>0.49</v>
       </c>
-      <c r="Y2" s="5">
-        <v>0</v>
+      <c r="Y2" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>49.2</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>3.89</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>15.3</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>13.7</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.15</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>3.88</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>3.88</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>6.76</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>3.44</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <v>1.22</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="4">
-        <v>0</v>
-      </c>
-      <c r="N3" s="4">
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
         <v>3.5</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="3">
         <v>1333</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="4">
         <v>56.5</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="Q3" s="4">
         <v>0.12</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="4">
         <v>26.9</v>
       </c>
-      <c r="S3" s="5">
+      <c r="S3" s="4">
         <v>0.47</v>
       </c>
-      <c r="T3" s="5">
-        <v>0</v>
-      </c>
-      <c r="U3" s="5">
+      <c r="T3" s="4">
+        <v>0</v>
+      </c>
+      <c r="U3" s="4">
         <v>0.05</v>
       </c>
-      <c r="V3" s="5">
+      <c r="V3" s="4">
         <v>8.9499999999999993</v>
       </c>
-      <c r="W3" s="5">
+      <c r="W3" s="4">
         <v>5.66</v>
       </c>
-      <c r="X3" s="5">
+      <c r="X3" s="4">
         <v>0.47</v>
       </c>
-      <c r="Y3" s="5">
-        <v>0</v>
+      <c r="Y3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>49.6</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>3.79</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>15.8</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>13</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>0.15</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>4.26</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>4.26</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>6.59</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>3.65</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>1.04</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>0.02</v>
       </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="4">
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
         <v>4</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="3">
         <v>1440</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="4">
         <v>57.6</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="Q4" s="4">
         <v>0.11</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="4">
         <v>26.3</v>
       </c>
-      <c r="S4" s="5">
+      <c r="S4" s="4">
         <v>0.5</v>
       </c>
-      <c r="T4" s="5">
-        <v>0</v>
-      </c>
-      <c r="U4" s="5">
+      <c r="T4" s="4">
+        <v>0</v>
+      </c>
+      <c r="U4" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V4" s="5">
+      <c r="V4" s="4">
         <v>8.5</v>
       </c>
-      <c r="W4" s="5">
+      <c r="W4" s="4">
         <v>6.27</v>
       </c>
-      <c r="X4" s="5">
+      <c r="X4" s="4">
         <v>0.4</v>
       </c>
-      <c r="Y4" s="5">
-        <v>0</v>
+      <c r="Y4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3">
+        <v>49.6</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3.79</v>
+      </c>
+      <c r="D5" s="3">
+        <v>15.8</v>
+      </c>
+      <c r="E5" s="3">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="G5" s="3">
+        <v>4.26</v>
+      </c>
+      <c r="H5" s="3">
+        <v>4.26</v>
+      </c>
+      <c r="I5" s="3">
+        <v>6.59</v>
+      </c>
+      <c r="J5" s="3">
+        <v>3.65</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1.04</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>4</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1440</v>
+      </c>
+      <c r="P5" s="4">
+        <v>57.6</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="R5" s="4">
+        <v>26.3</v>
+      </c>
+      <c r="S5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="T5" s="4">
+        <v>0</v>
+      </c>
+      <c r="U5" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V5" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="W5" s="4">
+        <v>6.27</v>
+      </c>
+      <c r="X5" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5">
+        <f>B5+0.1</f>
+        <v>49.7</v>
+      </c>
+      <c r="C6">
+        <f>C5-0.1</f>
+        <v>3.69</v>
+      </c>
+      <c r="D6">
+        <f>D5+0.1</f>
+        <v>15.9</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" ref="E6" si="0">E5+0.1</f>
+        <v>13.1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6" si="1">F5-0.1</f>
+        <v>4.9999999999999989E-2</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:H6" si="2">G5+0.1</f>
+        <v>4.3599999999999994</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" si="2"/>
+        <v>4.3599999999999994</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6" si="3">I5-0.1</f>
+        <v>6.49</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:K6" si="4">J5+0.1</f>
+        <v>3.75</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" si="4"/>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6:N6" si="5">M5+0.1</f>
+        <v>0.1</v>
+      </c>
+      <c r="N6" s="5">
+        <f t="shared" si="5"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6" si="6">O5-0.1</f>
+        <v>1439.9</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6:Q6" si="7">P5+0.1</f>
+        <v>57.7</v>
+      </c>
+      <c r="Q6" s="5">
+        <f t="shared" si="7"/>
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6" si="8">R5-0.1</f>
+        <v>26.2</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6:T6" si="9">S5+0.1</f>
+        <v>0.6</v>
+      </c>
+      <c r="T6" s="5">
+        <f t="shared" si="9"/>
+        <v>0.1</v>
+      </c>
+      <c r="U6">
+        <f t="shared" ref="U6" si="10">U5-0.1</f>
+        <v>-0.03</v>
+      </c>
+      <c r="V6">
+        <f t="shared" ref="V6:W6" si="11">V5+0.1</f>
+        <v>8.6</v>
+      </c>
+      <c r="W6" s="5">
+        <f t="shared" si="11"/>
+        <v>6.3699999999999992</v>
+      </c>
+      <c r="X6">
+        <f t="shared" ref="X6" si="12">X5-0.1</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" ref="Y6" si="13">Y5+0.1</f>
+        <v>0.1</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5">
+        <f>B6+0.1</f>
+        <v>49.800000000000004</v>
+      </c>
+      <c r="C7">
+        <f>C6-0.1</f>
+        <v>3.59</v>
+      </c>
+      <c r="D7">
+        <f>D6+0.1</f>
+        <v>16</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" ref="E7" si="14">E6+0.1</f>
+        <v>13.2</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7" si="15">F6-0.1</f>
+        <v>-5.0000000000000017E-2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7" si="16">G6+0.1</f>
+        <v>4.4599999999999991</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" ref="H7" si="17">H6+0.1</f>
+        <v>4.4599999999999991</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7" si="18">I6-0.1</f>
+        <v>6.3900000000000006</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7" si="19">J6+0.1</f>
+        <v>3.85</v>
+      </c>
+      <c r="K7" s="5">
+        <f t="shared" ref="K7" si="20">K6+0.1</f>
+        <v>1.2400000000000002</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ref="M7" si="21">M6+0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" ref="N7" si="22">N6+0.1</f>
+        <v>4.1999999999999993</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7" si="23">O6-0.1</f>
+        <v>1439.8000000000002</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ref="P7" si="24">P6+0.1</f>
+        <v>57.800000000000004</v>
+      </c>
+      <c r="Q7" s="5">
+        <f t="shared" ref="Q7" si="25">Q6+0.1</f>
+        <v>0.31000000000000005</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ref="R7" si="26">R6-0.1</f>
+        <v>26.099999999999998</v>
+      </c>
+      <c r="S7">
+        <f t="shared" ref="S7" si="27">S6+0.1</f>
+        <v>0.7</v>
+      </c>
+      <c r="T7" s="5">
+        <f t="shared" ref="T7" si="28">T6+0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="U7">
+        <f t="shared" ref="U7" si="29">U6-0.1</f>
+        <v>-0.13</v>
+      </c>
+      <c r="V7">
+        <f t="shared" ref="V7" si="30">V6+0.1</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="W7" s="5">
+        <f t="shared" ref="W7" si="31">W6+0.1</f>
+        <v>6.4699999999999989</v>
+      </c>
+      <c r="X7">
+        <f t="shared" ref="X7" si="32">X6-0.1</f>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" ref="Y7" si="33">Y6+0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>